<commit_message>
added test for reporte
</commit_message>
<xml_diff>
--- a/data/stock.xlsx
+++ b/data/stock.xlsx
@@ -263,6 +263,7 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -351,12 +352,12 @@
   <dimension ref="A1:F30"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="F17" activeCellId="0" sqref="F17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="12.55"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="12.56"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="12.41"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="30.33"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="17.83"/>

</xml_diff>